<commit_message>
second version with PTV window
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/check_protocol/ORL2-ne-pas-utiliser.xlsx
+++ b/Plancheck/plancheck_data/check_protocol/ORL2-ne-pas-utiliser.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="196">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -298,9 +298,6 @@
     <t>oui</t>
   </si>
   <si>
-    <t>D95%&gt;95%</t>
-  </si>
-  <si>
     <t>D0,1cc&lt;59Gy</t>
   </si>
   <si>
@@ -608,6 +605,12 @@
   </si>
   <si>
     <t>PTV_AUTRES</t>
+  </si>
+  <si>
+    <t>D98%&gt;95%</t>
+  </si>
+  <si>
+    <t>D97%&gt;95%</t>
   </si>
 </sst>
 </file>
@@ -1597,7 +1600,7 @@
   </sheetPr>
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1620,7 +1623,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
@@ -2049,7 +2052,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
@@ -2081,7 +2084,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B32" s="27">
         <v>0.125</v>
@@ -2098,7 +2101,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B33" s="27">
         <v>0.125</v>
@@ -2115,7 +2118,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>5</v>
@@ -2132,7 +2135,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B35" s="27" t="s">
         <v>6</v>
@@ -2232,7 +2235,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B44" s="23" t="s">
         <v>65</v>
@@ -2246,7 +2249,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B45" s="23">
         <v>300</v>
@@ -2260,7 +2263,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B46" s="23">
         <v>3</v>
@@ -2274,7 +2277,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B47" s="23">
         <v>100</v>
@@ -2288,7 +2291,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B48" s="23">
         <v>30</v>
@@ -2305,7 +2308,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B49" s="23">
         <v>0.1</v>
@@ -2332,37 +2335,37 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L55" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L56" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L57" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L58" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L59" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L60" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L61" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2427,59 +2430,59 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2494,26 +2497,26 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2522,92 +2525,92 @@
         <v>Oesophage</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2645,170 +2648,170 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2899,8 +2902,8 @@
   </sheetPr>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2951,96 +2954,96 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>91</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" t="s">
         <v>177</v>
-      </c>
-      <c r="B6" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12"/>
@@ -3049,59 +3052,59 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -3110,72 +3113,72 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" t="s">
         <v>184</v>
-      </c>
-      <c r="C25" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>